<commit_message>
Fix times for Jo (full precision)
</commit_message>
<xml_diff>
--- a/data/2020-03-03/Senior Cubers Worldwide - Weekly Competition - 2020-03-03.xlsx
+++ b/data/2020-03-03/Senior Cubers Worldwide - Weekly Competition - 2020-03-03.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-03-03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E5BA6C-7590-442A-99F6-A744ABF158CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB8D44F-ACE1-4252-B78E-F9506FBDB93F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -549,12 +549,6 @@
     <t>Shawn Boucké</t>
   </si>
   <si>
-    <t>1:03.00</t>
-  </si>
-  <si>
-    <t>1:30.00</t>
-  </si>
-  <si>
     <t>🏆 ⚡</t>
   </si>
   <si>
@@ -562,6 +556,12 @@
   </si>
   <si>
     <t>⚡</t>
+  </si>
+  <si>
+    <t>1:03.61</t>
+  </si>
+  <si>
+    <t>1:30.63</t>
   </si>
 </sst>
 </file>
@@ -711,7 +711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -869,6 +869,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1090,7 +1093,7 @@
   <dimension ref="A1:M1074"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2073,25 +2076,25 @@
         <v>16</v>
       </c>
       <c r="D28" s="45">
-        <v>58</v>
-      </c>
-      <c r="E28" s="45">
-        <v>51</v>
+        <v>58.76</v>
+      </c>
+      <c r="E28" s="46">
+        <v>51.24</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>147</v>
       </c>
       <c r="G28" s="46">
-        <v>57</v>
+        <v>57.82</v>
       </c>
       <c r="H28" s="46">
-        <v>51</v>
+        <v>51.24</v>
       </c>
       <c r="I28" s="64" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="J28" s="64" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="K28" s="46">
         <v>54.84</v>
@@ -2102,6 +2105,7 @@
     </row>
     <row r="29" spans="1:12" ht="12.75">
       <c r="A29" s="20"/>
+      <c r="I29" s="67"/>
     </row>
     <row r="30" spans="1:12" ht="12.75">
       <c r="A30" s="20"/>
@@ -14765,7 +14769,7 @@
         <v>36</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G4" s="23" t="s">
         <v>58</v>
@@ -23660,7 +23664,7 @@
         <v>26</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G5" s="15" t="s">
         <v>25</v>
@@ -23724,7 +23728,7 @@
         <v>17</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Add 2020-03-24 and rename Tim Salay to Timothy Salay
</commit_message>
<xml_diff>
--- a/data/2020-03-03/Senior Cubers Worldwide - Weekly Competition - 2020-03-03.xlsx
+++ b/data/2020-03-03/Senior Cubers Worldwide - Weekly Competition - 2020-03-03.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-03-03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89AABEA-12D1-4313-89C4-71A198E78218}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7F496B-57DA-4676-9482-0365B7A4243E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -441,9 +441,6 @@
     <t>https://www.facebook.com/events/241721610185997/permalink/243337186691106/</t>
   </si>
   <si>
-    <t>Tim Salay</t>
-  </si>
-  <si>
     <t>https://www.facebook.com/events/241721610185997/permalink/242622543429237/</t>
   </si>
   <si>
@@ -562,6 +559,9 @@
   </si>
   <si>
     <t>Raimon Schaap</t>
+  </si>
+  <si>
+    <t>Timothy Salay</t>
   </si>
 </sst>
 </file>
@@ -870,9 +870,9 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1094,7 +1094,7 @@
   <dimension ref="A1:M1074"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1412,8 +1412,8 @@
       <c r="A10" s="20">
         <v>7</v>
       </c>
-      <c r="B10" s="68" t="s">
-        <v>176</v>
+      <c r="B10" s="66" t="s">
+        <v>175</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>78</v>
@@ -1777,7 +1777,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>47</v>
@@ -1805,7 +1805,7 @@
         <v>35.31</v>
       </c>
       <c r="L20" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="12.75">
@@ -1849,7 +1849,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>136</v>
+        <v>176</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>16</v>
@@ -1877,7 +1877,7 @@
         <v>37.29</v>
       </c>
       <c r="L22" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="12.75">
@@ -1885,7 +1885,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>47</v>
@@ -1913,7 +1913,7 @@
         <v>32.31</v>
       </c>
       <c r="L23" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="12.75">
@@ -1921,7 +1921,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="62" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>16</v>
@@ -1951,7 +1951,7 @@
         <v>27.78</v>
       </c>
       <c r="L24" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="12.75">
@@ -1959,7 +1959,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>16</v>
@@ -1987,7 +1987,7 @@
         <v>29.42</v>
       </c>
       <c r="L25" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="12.75">
@@ -1995,7 +1995,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>47</v>
@@ -2007,7 +2007,7 @@
         <v>35.409999999999997</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G26" s="17">
         <v>36.36</v>
@@ -2025,7 +2025,7 @@
         <v>46.28</v>
       </c>
       <c r="L26" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="12.75">
@@ -2060,10 +2060,10 @@
         <v>39.4</v>
       </c>
       <c r="K27" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="L27" s="18" t="s">
         <v>148</v>
-      </c>
-      <c r="L27" s="18" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="12.75">
@@ -2071,7 +2071,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C28" s="21" t="s">
         <v>16</v>
@@ -2083,7 +2083,7 @@
         <v>51.24</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G28" s="46">
         <v>57.82</v>
@@ -2092,16 +2092,16 @@
         <v>51.24</v>
       </c>
       <c r="I28" s="64" t="s">
+        <v>173</v>
+      </c>
+      <c r="J28" s="64" t="s">
         <v>174</v>
-      </c>
-      <c r="J28" s="64" t="s">
-        <v>175</v>
       </c>
       <c r="K28" s="46">
         <v>54.84</v>
       </c>
       <c r="L28" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="12.75">
@@ -14770,7 +14770,7 @@
         <v>36</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G4" s="23" t="s">
         <v>58</v>
@@ -23665,7 +23665,7 @@
         <v>26</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G5" s="15" t="s">
         <v>25</v>
@@ -23729,7 +23729,7 @@
         <v>17</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>17</v>
@@ -30258,14 +30258,14 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="53" t="s">
-        <v>152</v>
-      </c>
-      <c r="B1" s="66" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
       <c r="F1" s="54"/>
     </row>
     <row r="2" spans="1:7" ht="12.75">
@@ -30287,16 +30287,16 @@
         <v>6</v>
       </c>
       <c r="D3" s="57" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E3" s="57" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="G3" s="59" t="s">
         <v>154</v>
-      </c>
-      <c r="G3" s="59" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="12.75">
@@ -30304,7 +30304,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>47</v>
@@ -30316,7 +30316,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="60" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="12.75">
@@ -30324,7 +30324,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C5" s="50" t="s">
         <v>16</v>
@@ -30336,7 +30336,7 @@
         <v>27</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="12.75">
@@ -30344,7 +30344,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>121</v>
@@ -30354,7 +30354,7 @@
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="60" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="12.75">
@@ -30362,7 +30362,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C7" s="50" t="s">
         <v>47</v>
@@ -30371,10 +30371,10 @@
         <v>30</v>
       </c>
       <c r="E7" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="F7" s="60" t="s">
         <v>162</v>
-      </c>
-      <c r="F7" s="60" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="12.75">
@@ -30382,7 +30382,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C8" s="50" t="s">
         <v>121</v>
@@ -30392,7 +30392,7 @@
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="60" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="12.75">
@@ -30409,10 +30409,10 @@
         <v>45</v>
       </c>
       <c r="F9" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="G9" s="14" t="s">
         <v>166</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="12.75">
@@ -30429,7 +30429,7 @@
         <v>48</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="12.75">

</xml_diff>

<commit_message>
FIx incorrect best times
</commit_message>
<xml_diff>
--- a/data/2020-03-03/Senior Cubers Worldwide - Weekly Competition - 2020-03-03.xlsx
+++ b/data/2020-03-03/Senior Cubers Worldwide - Weekly Competition - 2020-03-03.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-03-03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78526E44-6B65-4438-B8BC-BEDC9D6288DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B471A26-C849-4132-9F8C-D4323E2F5DD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3x3x3" sheetId="1" r:id="rId1"/>
@@ -1093,7 +1093,7 @@
   </sheetPr>
   <dimension ref="A1:M1074"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -14666,8 +14666,8 @@
   </sheetPr>
   <dimension ref="A1:M1044"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -14881,7 +14881,7 @@
         <v>86</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>88</v>

</xml_diff>